<commit_message>
Ajuste link do Trello
</commit_message>
<xml_diff>
--- a/Backlog/Backlog.xlsx
+++ b/Backlog/Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D4A66E-9EEB-4A3A-B4BD-18C7C8BFF231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4893742B-E2A8-4D4E-803F-24661552078E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -289,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -309,15 +309,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,547 +322,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -949,7 +400,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -989,12 +445,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1098,18 +549,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:E40" totalsRowShown="0" headerRowDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:E40" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A2:E40" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E40">
     <sortCondition ref="E3:E40"/>
     <sortCondition ref="D3:D40"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Descrição" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Situação" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{FB961424-78DB-4B77-AA3E-E371EBCFF2CC}" name="Matéria" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{815EDD6F-9FD8-4082-8044-EDB9B713480C}" name="Sprint" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Descrição" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Situação" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{FB961424-78DB-4B77-AA3E-E371EBCFF2CC}" name="Matéria" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{815EDD6F-9FD8-4082-8044-EDB9B713480C}" name="Sprint" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1380,30 +831,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="87" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -1420,7 +871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1437,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1471,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1488,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1505,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1522,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1540,7 +991,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1557,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1574,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1591,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -1608,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1625,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -1642,7 +1093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
@@ -1659,7 +1110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -1676,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -1693,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -1710,7 +1161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
@@ -1727,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -1744,7 +1195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
@@ -1761,7 +1212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
@@ -1778,7 +1229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
@@ -1795,7 +1246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1812,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1829,7 +1280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -1846,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -1863,7 +1314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
@@ -1880,7 +1331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -1888,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>41</v>
@@ -1897,7 +1348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
@@ -1914,11 +1365,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1927,15 +1378,15 @@
       <c r="D32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1944,15 +1395,15 @@
       <c r="D33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1961,15 +1412,15 @@
       <c r="D34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1978,15 +1429,15 @@
       <c r="D35" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1995,15 +1446,15 @@
       <c r="D36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -2012,15 +1463,15 @@
       <c r="D37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -2029,15 +1480,15 @@
       <c r="D38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="7" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -2046,15 +1497,15 @@
       <c r="D39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -2063,7 +1514,7 @@
       <c r="D40" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="1">
         <v>3</v>
       </c>
     </row>
@@ -2072,24 +1523,24 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:D40">
-    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Desejável"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D40">
-    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Alterações no Backlog na coluna Descrição
</commit_message>
<xml_diff>
--- a/Backlog/Backlog.xlsx
+++ b/Backlog/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA933DB7-B8FB-4F4E-820E-EB948645C114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2A28DE-D17C-4D39-BB07-1BDF3CCC2ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="94">
   <si>
     <t>Configuração e instalação do Arduino Uno R3 com Sensor MQ-2 utilizando Protoboard e 3 Jumpers (Macho-Macho).</t>
   </si>
@@ -247,6 +247,99 @@
   </si>
   <si>
     <t>Tornar o Site Responsivo</t>
+  </si>
+  <si>
+    <t>Simulador Financeiro em HTML e JS que mostre o valor agregado da nossa empresa</t>
+  </si>
+  <si>
+    <t>Tabelas no MySQL que posteriormente irão armazenar os dados dos sensores e os dados de cadastro</t>
+  </si>
+  <si>
+    <t>Diagrama que mostra para o cliente como funciona o nosso negócio de maneira simples e intuitiva, não técnica</t>
+  </si>
+  <si>
+    <t>Documentação do Projeto como um todo, contendo: Capa, Sumário, Contexto, Objetivo, Justificativa, Escopo, Premissas, Restrições e Referências Bibliográficas</t>
+  </si>
+  <si>
+    <t>Repositório no Git onde serão armazenados todos os arquivos que farão parte desse projeto</t>
+  </si>
+  <si>
+    <t>Trello, configurá-lo para que a equipe possa acompanhar o andamento das atividades</t>
+  </si>
+  <si>
+    <t>Configurar o Arduíno, incluindo montagem física do sensor e programação via Arduino IDE</t>
+  </si>
+  <si>
+    <t>Instalar o Linux na VM para posteriormente testarmos e alocarmos a nossa aplicação</t>
+  </si>
+  <si>
+    <t>Protótipo do Site no Figma, Canva ou Photoshop para mostrar ao cliente como será o site</t>
+  </si>
+  <si>
+    <t>Dashboard via Arduino IDE onde serão plotados os dados dos sensores</t>
+  </si>
+  <si>
+    <t>Inserts e Selects nas tabelas criadas acima para mostrar ao cliente</t>
+  </si>
+  <si>
+    <t>Comandos que criam usuários, diretórios e arquivos para o cliente na VM</t>
+  </si>
+  <si>
+    <t>Máscarar os inputs para facilitar o Insert dos dados no banco e a utilização do usuário</t>
+  </si>
+  <si>
+    <t>Criptografar as senhas inseridos no cadastro do usuário quando enviadas para o banco de dados</t>
+  </si>
+  <si>
+    <t>Telas de Cadastro e Login em HTML, CSS e JS, mas que ainda não enviarão dados para o banco</t>
+  </si>
+  <si>
+    <t>Site estático em HTML, CSS e JS que seguirá o protótipo já montado</t>
+  </si>
+  <si>
+    <t>Site em HTML, CSS e JS que terá a integração com o Arduíno, mostrando os dados do sensor em forma de gráficos</t>
+  </si>
+  <si>
+    <t>Modelagem Lógica que irá conter as tabelas do banco de dados e o seu relacionamento</t>
+  </si>
+  <si>
+    <t>Criar novamente as tabelas, mas dessa vez adicionar as chaves estrangeiras e o relacionamento</t>
+  </si>
+  <si>
+    <t>Atualização do projeto no GitHub</t>
+  </si>
+  <si>
+    <t>Atualização da documentação para rever os detalhes que precisam ser melhorado mediam o feedback do cliente e a Sprint Review</t>
+  </si>
+  <si>
+    <t>Organizar as atividades novamente no Trello</t>
+  </si>
+  <si>
+    <t>Adicionar mais três colunas ao Backlog: Tamanho, Prioridade e Responsável</t>
+  </si>
+  <si>
+    <t>Utilizar a API para simular a Dashboard juntamente com os dados vindo do Arduíno</t>
+  </si>
+  <si>
+    <t>Teste da API no localhost</t>
+  </si>
+  <si>
+    <t>Utilização do MySQL na VM com o objetivo de isolar o ambiente da aplicação</t>
+  </si>
+  <si>
+    <t>Diagrama que mostrará uma visão técnica da nossa solução</t>
+  </si>
+  <si>
+    <t>Validar o Diagrama de Solução</t>
+  </si>
+  <si>
+    <t>Elaborar a planilha de riscos do nosso projeto</t>
+  </si>
+  <si>
+    <t>Especificar qual será a dashboard utilizada para exibir os dados para o cliente</t>
+  </si>
+  <si>
+    <t>Montar um sistema de recuperação de senhas no nosso site</t>
   </si>
 </sst>
 </file>
@@ -330,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -360,12 +453,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -676,8 +763,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:I43" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A2:I43" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I43">
+    <sortCondition ref="G3:G43"/>
+    <sortCondition ref="C3:C43"/>
     <sortCondition ref="F3:F43"/>
-    <sortCondition ref="I3:I43"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="14"/>
@@ -961,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K4:K7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1024,7 +1112,9 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1048,11 +1138,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1076,11 +1168,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1104,11 +1198,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1132,11 +1228,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1161,11 +1259,13 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1193,7 +1293,9 @@
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1222,7 +1324,9 @@
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1246,11 +1350,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1278,7 +1384,9 @@
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1306,7 +1414,9 @@
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1334,7 +1444,9 @@
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1358,20 +1470,22 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="str" cm="1">
         <f t="array" ref="D15">_xlfn.IFS(E15=3,"PP",E15=5,"P",E15=8,"M",E15=13,"G",E15=21,"GG")</f>
-        <v>G</v>
+        <v>P</v>
       </c>
       <c r="E15" s="6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F15" s="6">
         <v>3</v>
@@ -1386,20 +1500,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="2" t="str" cm="1">
         <f t="array" ref="D16">_xlfn.IFS(E16=3,"PP",E16=5,"P",E16=8,"M",E16=13,"G",E16=21,"GG")</f>
-        <v>P</v>
+        <v>PP</v>
       </c>
       <c r="E16" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="6">
         <v>3</v>
@@ -1411,14 +1527,16 @@
         <v>33</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
@@ -1442,11 +1560,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
@@ -1470,11 +1590,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1498,23 +1620,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="str" cm="1">
         <f t="array" ref="D20">_xlfn.IFS(E20=3,"PP",E20=5,"P",E20=8,"M",E20=13,"G",E20=21,"GG")</f>
-        <v>P</v>
+        <v>PP</v>
       </c>
       <c r="E20" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F20" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
         <v>2</v>
@@ -1523,44 +1647,48 @@
         <v>31</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="str" cm="1">
         <f t="array" ref="D21">_xlfn.IFS(E21=3,"PP",E21=5,"P",E21=8,"M",E21=13,"G",E21=21,"GG")</f>
-        <v>PP</v>
+        <v>P</v>
       </c>
       <c r="E21" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F21" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1">
         <v>2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="C22" s="2" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="str" cm="1">
         <f t="array" ref="D22">_xlfn.IFS(E22=3,"PP",E22=5,"P",E22=8,"M",E22=13,"G",E22=21,"GG")</f>
@@ -1570,32 +1698,34 @@
         <v>3</v>
       </c>
       <c r="F22" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1">
         <v>2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="str" cm="1">
         <f t="array" ref="D23">_xlfn.IFS(E23=3,"PP",E23=5,"P",E23=8,"M",E23=13,"G",E23=21,"GG")</f>
-        <v>PP</v>
+        <v>G</v>
       </c>
       <c r="E23" s="6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F23" s="6">
         <v>1</v>
@@ -1607,23 +1737,25 @@
         <v>31</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="str" cm="1">
         <f t="array" ref="D24">_xlfn.IFS(E24=3,"PP",E24=5,"P",E24=8,"M",E24=13,"G",E24=21,"GG")</f>
-        <v>P</v>
+        <v>PP</v>
       </c>
       <c r="E24" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F24" s="6">
         <v>1</v>
@@ -1632,29 +1764,31 @@
         <v>2</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="str" cm="1">
         <f t="array" ref="D25">_xlfn.IFS(E25=3,"PP",E25=5,"P",E25=8,"M",E25=13,"G",E25=21,"GG")</f>
-        <v>PP</v>
+        <v>P</v>
       </c>
       <c r="E25" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F25" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1">
         <v>2</v>
@@ -1663,14 +1797,16 @@
         <v>31</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>1</v>
       </c>
@@ -1682,23 +1818,25 @@
         <v>5</v>
       </c>
       <c r="F26" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="C27" s="2" t="s">
         <v>1</v>
       </c>
@@ -1710,35 +1848,37 @@
         <v>3</v>
       </c>
       <c r="F27" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" s="1">
         <v>2</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="C28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="str" cm="1">
         <f t="array" ref="D28">_xlfn.IFS(E28=3,"PP",E28=5,"P",E28=8,"M",E28=13,"G",E28=21,"GG")</f>
-        <v>G</v>
+        <v>PP</v>
       </c>
       <c r="E28" s="6">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F28" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="1">
         <v>2</v>
@@ -1747,14 +1887,16 @@
         <v>31</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="C29" s="2" t="s">
         <v>1</v>
       </c>
@@ -1766,7 +1908,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="1">
         <v>2</v>
@@ -1775,14 +1917,16 @@
         <v>33</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
       </c>
@@ -1803,14 +1947,16 @@
         <v>33</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>1</v>
       </c>
@@ -1822,7 +1968,7 @@
         <v>8</v>
       </c>
       <c r="F31" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31" s="1">
         <v>2</v>
@@ -1831,96 +1977,100 @@
         <v>33</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="str" cm="1">
         <f t="array" ref="D32">_xlfn.IFS(E32=3,"PP",E32=5,"P",E32=8,"M",E32=13,"G",E32=21,"GG")</f>
-        <v>PP</v>
+        <v>P</v>
       </c>
       <c r="E32" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F32" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G32" s="1">
         <v>2</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="C33" s="2" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D33" s="2" t="str" cm="1">
         <f t="array" ref="D33">_xlfn.IFS(E33=3,"PP",E33=5,"P",E33=8,"M",E33=13,"G",E33=21,"GG")</f>
-        <v>P</v>
+        <v>G</v>
       </c>
       <c r="E33" s="6">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F33" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G33" s="1">
         <v>2</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
-        <v>62</v>
+      <c r="A34" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="12" t="s">
-        <v>35</v>
+      <c r="C34" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D34" s="2" t="str" cm="1">
         <f t="array" ref="D34">_xlfn.IFS(E34=3,"PP",E34=5,"P",E34=8,"M",E34=13,"G",E34=21,"GG")</f>
-        <v>G</v>
+        <v>P</v>
       </c>
       <c r="E34" s="6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F34" s="6">
-        <v>3</v>
-      </c>
-      <c r="G34" s="6">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
         <v>3</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="2" t="s">
@@ -1928,13 +2078,13 @@
       </c>
       <c r="D35" s="2" t="str" cm="1">
         <f t="array" ref="D35">_xlfn.IFS(E35=3,"PP",E35=5,"P",E35=8,"M",E35=13,"G",E35=21,"GG")</f>
-        <v>M</v>
+        <v>P</v>
       </c>
       <c r="E35" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F35" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G35" s="1">
         <v>3</v>
@@ -1943,12 +2093,12 @@
         <v>33</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="2" t="s">
@@ -1956,13 +2106,13 @@
       </c>
       <c r="D36" s="2" t="str" cm="1">
         <f t="array" ref="D36">_xlfn.IFS(E36=3,"PP",E36=5,"P",E36=8,"M",E36=13,"G",E36=21,"GG")</f>
-        <v>M</v>
+        <v>G</v>
       </c>
       <c r="E36" s="6">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F36" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G36" s="1">
         <v>3</v>
@@ -1971,12 +2121,12 @@
         <v>33</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="2" t="s">
@@ -1984,13 +2134,13 @@
       </c>
       <c r="D37" s="2" t="str" cm="1">
         <f t="array" ref="D37">_xlfn.IFS(E37=3,"PP",E37=5,"P",E37=8,"M",E37=13,"G",E37=21,"GG")</f>
-        <v>P</v>
+        <v>M</v>
       </c>
       <c r="E37" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F37" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G37" s="1">
         <v>3</v>
@@ -1999,12 +2149,12 @@
         <v>33</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="2" t="s">
@@ -2032,7 +2182,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="2" t="s">
@@ -2040,13 +2190,13 @@
       </c>
       <c r="D39" s="2" t="str" cm="1">
         <f t="array" ref="D39">_xlfn.IFS(E39=3,"PP",E39=5,"P",E39=8,"M",E39=13,"G",E39=21,"GG")</f>
-        <v>P</v>
+        <v>M</v>
       </c>
       <c r="E39" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F39" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G39" s="1">
         <v>3</v>
@@ -2055,12 +2205,12 @@
         <v>33</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="2" t="s">
@@ -2074,7 +2224,7 @@
         <v>5</v>
       </c>
       <c r="F40" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40" s="1">
         <v>3</v>
@@ -2083,12 +2233,12 @@
         <v>33</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="2" t="s">
@@ -2102,7 +2252,7 @@
         <v>8</v>
       </c>
       <c r="F41" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G41" s="1">
         <v>3</v>
@@ -2111,7 +2261,7 @@
         <v>33</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -2144,11 +2294,11 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="2" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D43" s="2" t="str" cm="1">
         <f t="array" ref="D43">_xlfn.IFS(E43=3,"PP",E43=5,"P",E43=8,"M",E43=13,"G",E43=21,"GG")</f>
@@ -2158,16 +2308,16 @@
         <v>13</v>
       </c>
       <c r="F43" s="6">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="6">
         <v>3</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>